<commit_message>
Inserita la visualizzazione della data ma sto facendo ancora prove su prove per inserire le celle colorate, quello è un bel casino
</commit_message>
<xml_diff>
--- a/windows_form_app/SpreadsheetDocumentEx.xlsx
+++ b/windows_form_app/SpreadsheetDocumentEx.xlsx
@@ -1,14 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TEST" sheetId="1" r:id="Rcee5fdb8fd304e38"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TEST" sheetId="1" r:id="Rf5b6599f34d04874"/>
   </x:sheets>
 </x:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:si>
+    <x:t>30/12/2018</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetData/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetData>
+    <x:row r="2">
+      <x:c r="B2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="1">
+      <x:c r="B1"/>
+      <x:c r="H1"/>
+      <x:c r="I1"/>
+      <x:c r="O1"/>
+      <x:c r="P1"/>
+      <x:c r="V1"/>
+    </x:row>
+  </x:sheetData>
+  <x:mergeCells>
+    <x:mergeCell ref="B1:H1"/>
+    <x:mergeCell ref="I1:O1"/>
+    <x:mergeCell ref="P1:V1"/>
+  </x:mergeCells>
+</x:worksheet>
 </file>
</xml_diff>